<commit_message>
half of the amazon data.
</commit_message>
<xml_diff>
--- a/google_summary.xlsx
+++ b/google_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/narijohnson/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D74931-53F3-B542-AFB8-692AE58643AF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C946477D-FEB4-4048-B28A-EF8B39FB2E39}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21080" yWindow="460" windowWidth="16560" windowHeight="15440" xr2:uid="{488B5631-6CC4-F74F-AFC3-02386379F48D}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Category</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>accuracy stdev</t>
+  </si>
+  <si>
+    <t>accuracy RATE mean</t>
   </si>
 </sst>
 </file>
@@ -438,15 +441,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64CAD98C-EB11-6E42-9211-8FBB1814DA87}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,10 +467,13 @@
         <v>15</v>
       </c>
       <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -477,10 +487,14 @@
         <v>17.133299999999998</v>
       </c>
       <c r="E2">
+        <f xml:space="preserve"> $D2 / 69</f>
+        <v>0.24830869565217389</v>
+      </c>
+      <c r="F2">
         <v>13.85</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -494,10 +508,14 @@
         <v>15.266999999999999</v>
       </c>
       <c r="E3">
+        <f t="shared" ref="E3:E15" si="0" xml:space="preserve"> $D3 / 69</f>
+        <v>0.22126086956521737</v>
+      </c>
+      <c r="F3">
         <v>11.627000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -511,10 +529,14 @@
         <v>25.533300000000001</v>
       </c>
       <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0.37004782608695652</v>
+      </c>
+      <c r="F4">
         <v>16.724</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -528,10 +550,14 @@
         <v>7.4667000000000003</v>
       </c>
       <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.10821304347826087</v>
+      </c>
+      <c r="F5">
         <v>8.4250000000000007</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -545,10 +571,14 @@
         <v>11.333</v>
       </c>
       <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.16424637681159421</v>
+      </c>
+      <c r="F6">
         <v>7.907</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -562,10 +592,14 @@
         <v>12.333</v>
       </c>
       <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.17873913043478262</v>
+      </c>
+      <c r="F7">
         <v>8.0060000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -579,10 +613,14 @@
         <v>24.2</v>
       </c>
       <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.35072463768115941</v>
+      </c>
+      <c r="F8">
         <v>18.882999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -596,10 +634,14 @@
         <v>14.8666</v>
       </c>
       <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.21545797101449277</v>
+      </c>
+      <c r="F9">
         <v>14.257</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -613,10 +655,14 @@
         <v>19.600000000000001</v>
       </c>
       <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.28405797101449276</v>
+      </c>
+      <c r="F10">
         <v>11.280799999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -630,10 +676,14 @@
         <v>13.8</v>
       </c>
       <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="F11">
         <v>7.5327000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -647,10 +697,14 @@
         <v>33.6</v>
       </c>
       <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.48695652173913045</v>
+      </c>
+      <c r="F12">
         <v>59.18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -664,10 +718,14 @@
         <v>18.133299999999998</v>
       </c>
       <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0.26280144927536231</v>
+      </c>
+      <c r="F13">
         <v>8.3054000000000006</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -681,10 +739,14 @@
         <v>9.5333000000000006</v>
       </c>
       <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.13816376811594203</v>
+      </c>
+      <c r="F14">
         <v>8.5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -698,6 +760,10 @@
         <v>29.533000000000001</v>
       </c>
       <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0.42801449275362319</v>
+      </c>
+      <c r="F15">
         <v>11.67</v>
       </c>
     </row>

</xml_diff>